<commit_message>
hydropower disaggregation, base case fix
</commit_message>
<xml_diff>
--- a/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
+++ b/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasinsari/Documents/AILabProject/PythonTest/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a0351697a6effba/Documenten/MASTER/Year 2/THESIS/16.02.22.Multiobjective/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B6C5F2-D355-AB4B-9FE7-C0306E5C2CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{D3B6C5F2-D355-AB4B-9FE7-C0306E5C2CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85A24F1F-4937-42AE-8CBF-57376A640351}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="540" windowWidth="28040" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1545" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelParameters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
   <si>
     <t>AttributeName</t>
   </si>
@@ -236,13 +236,25 @@
   </si>
   <si>
     <t>str</t>
+  </si>
+  <si>
+    <t>NobjHYD</t>
+  </si>
+  <si>
+    <t>Number of objective variables that the simulation outputs for the disaggregated objectives for hydropower production</t>
+  </si>
+  <si>
+    <t>NobjIRR</t>
+  </si>
+  <si>
+    <t>Number of objective variables that the simulation outputs for the disaggregated objectives for irrigation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,6 +407,12 @@
       <color rgb="FFCE9178"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -744,7 +762,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -768,6 +786,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -863,9 +884,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B4:E19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B4:E19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B4:E21" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="B4:E21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="AttributeName" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="8"/>
@@ -1186,25 +1211,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="4" customWidth="1"/>
-    <col min="2" max="3" width="40.83203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="39.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="45.83203125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="16.625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="40.875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="39.375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="45.875" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="24.95" customHeight="1"/>
+    <row r="2" spans="1:5" ht="24.95" customHeight="1"/>
+    <row r="3" spans="1:5" ht="24.95" customHeight="1"/>
+    <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
@@ -1221,7 +1246,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="31.5">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1235,7 +1260,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1249,7 +1274,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1263,7 +1288,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1277,7 +1302,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="31.5">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1291,7 +1316,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="47.25">
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1330,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1319,7 +1344,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1333,7 +1358,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1347,7 +1372,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
@@ -1361,7 +1386,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1375,7 +1400,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1389,7 +1414,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5">
       <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
@@ -1403,7 +1428,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5">
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
@@ -1417,7 +1442,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5">
       <c r="B19" s="7" t="s">
         <v>65</v>
       </c>
@@ -1426,6 +1451,34 @@
       </c>
       <c r="D19" s="4" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="47.25">
+      <c r="B20" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="9">
+        <v>8</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="31.5">
+      <c r="B21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="9">
+        <v>11</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1444,19 +1497,19 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="45.83203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="16.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="45.875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="24.95" customHeight="1"/>
+    <row r="2" spans="1:5" ht="24.95" customHeight="1"/>
+    <row r="3" spans="1:5" ht="24.95" customHeight="1"/>
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1473,7 +1526,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="31.5">
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1487,7 +1540,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1501,7 +1554,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="47.25">
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1515,7 +1568,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="47.25">
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1529,7 +1582,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1543,7 +1596,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="47.25">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1557,7 +1610,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="47.25">
       <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1571,7 +1624,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="63">
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1585,7 +1638,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="47.25">
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
@@ -1599,7 +1652,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="47.25">
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1613,7 +1666,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="47.25">
       <c r="B15" s="1" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
bc and irr 'done', hyd verification
</commit_message>
<xml_diff>
--- a/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
+++ b/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a0351697a6effba/Documenten/MASTER/Year 2/THESIS/16.02.22.Multiobjective/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{D3B6C5F2-D355-AB4B-9FE7-C0306E5C2CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F4537A5-8BD6-4F2F-A3C3-008FE1CA2D3E}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{D3B6C5F2-D355-AB4B-9FE7-C0306E5C2CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B14F7FA-3CBB-4C67-9429-D550BDC6F589}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="8370" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4950" yWindow="5865" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelParameters" sheetId="1" r:id="rId1"/>
@@ -888,6 +888,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1216,7 +1220,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -1309,7 +1313,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
opt_full settings = 16 obj
</commit_message>
<xml_diff>
--- a/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
+++ b/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a0351697a6effba/Documenten/MASTER/Year 2/THESIS/16.02.22.Multiobjective/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{D3B6C5F2-D355-AB4B-9FE7-C0306E5C2CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B14F7FA-3CBB-4C67-9429-D550BDC6F589}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{D3B6C5F2-D355-AB4B-9FE7-C0306E5C2CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C4CE648-D131-4D2C-98C2-C213723C253B}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="5865" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5385" yWindow="1545" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelParameters" sheetId="1" r:id="rId1"/>
@@ -1220,7 +1220,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -1313,7 +1313,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
HYD settings = 8 obj
</commit_message>
<xml_diff>
--- a/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
+++ b/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a0351697a6effba/Documenten/MASTER/Year 2/THESIS/16.02.22.Multiobjective/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{D3B6C5F2-D355-AB4B-9FE7-C0306E5C2CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D2A16A3-4CA5-45EF-87C3-813C0FF175D6}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{D3B6C5F2-D355-AB4B-9FE7-C0306E5C2CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28FFCB80-766F-4DA2-BE4D-D4CFC452756F}"/>
   <bookViews>
     <workbookView xWindow="5040" yWindow="1200" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -888,6 +888,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1216,7 +1220,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -1309,7 +1313,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
FULL settings = 16 obj
</commit_message>
<xml_diff>
--- a/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
+++ b/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a0351697a6effba/Documenten/MASTER/Year 2/THESIS/16.02.22.Multiobjective/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{D3B6C5F2-D355-AB4B-9FE7-C0306E5C2CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28FFCB80-766F-4DA2-BE4D-D4CFC452756F}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{D3B6C5F2-D355-AB4B-9FE7-C0306E5C2CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B63BC02F-5F8C-4F78-8126-248C78D32737}"/>
   <bookViews>
     <workbookView xWindow="5040" yWindow="1200" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
   <si>
     <t>AttributeName</t>
   </si>
@@ -250,17 +250,44 @@
     <t>Number of objective variables that the simulation outputs for the disaggregated objectives for environmental flow deficit</t>
   </si>
   <si>
-    <t>Number of objective variables that the simulation outputs for the disaggregated objectives for hydropower production deficit</t>
-  </si>
-  <si>
     <t>Number of objective variables that the simulation outputs for the disaggregated objectives for irrigation deficit</t>
+  </si>
+  <si>
+    <t>NobjFULL</t>
+  </si>
+  <si>
+    <t>Number of objective variables that the simulation outputs in the case of full disaggregation for both the hydropower and the irrigation case</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Number of objective variables that the simulation outputs for the disaggregated objectives for hydropower production deficit. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TO IMPLEMENT:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Change Nobj in row 9 above</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -415,6 +442,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -895,8 +929,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B4:E22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B4:E22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B4:E23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="B4:E23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="AttributeName" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="8"/>
@@ -1217,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -1313,7 +1347,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>4</v>
@@ -1459,7 +1493,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="47.25">
+    <row r="20" spans="2:5" ht="63">
       <c r="B20" s="9" t="s">
         <v>68</v>
       </c>
@@ -1470,7 +1504,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="47.25">
@@ -1484,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="47.25">
@@ -1499,6 +1533,20 @@
       </c>
       <c r="E22" s="9" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="47.25">
+      <c r="B23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="9">
+        <v>16</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simulation in progress, irr settings
</commit_message>
<xml_diff>
--- a/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
+++ b/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a0351697a6effba/Documenten/MASTER/Year 2/THESIS/16.02.22.Multiobjective/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{63EE93E9-248D-46C9-B53A-FBE29B5B3F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D2CAEE1-BA4B-4E39-9D67-35FDDAEBBC51}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{63EE93E9-248D-46C9-B53A-FBE29B5B3F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{781CE914-B99E-44F7-8B08-6F45F67DBA39}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelParameters" sheetId="1" r:id="rId1"/>
@@ -922,6 +922,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1249,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -1343,7 +1347,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
simulation in progress, full settings
</commit_message>
<xml_diff>
--- a/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
+++ b/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a0351697a6effba/Documenten/MASTER/Year 2/THESIS/16.02.22.Multiobjective/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{63EE93E9-248D-46C9-B53A-FBE29B5B3F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{781CE914-B99E-44F7-8B08-6F45F67DBA39}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{63EE93E9-248D-46C9-B53A-FBE29B5B3F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0343314A-3FE1-474C-B3F8-66C26B5E7453}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelParameters" sheetId="1" r:id="rId1"/>
@@ -1253,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B18" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1347,7 +1347,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
simulation in progress, bc settings
</commit_message>
<xml_diff>
--- a/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
+++ b/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/excel_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a0351697a6effba/Documenten/MASTER/Year 2/THESIS/16.02.22.Multiobjective/Multiobjective-multi-reservoir-control-d50e4da0f6a9a9c852b4904e640299adc96714bb/ZambeziSmashPython/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{63EE93E9-248D-46C9-B53A-FBE29B5B3F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0343314A-3FE1-474C-B3F8-66C26B5E7453}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{63EE93E9-248D-46C9-B53A-FBE29B5B3F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB11A9E3-3053-4559-B674-035A2DA274DA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30360" yWindow="2790" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelParameters" sheetId="1" r:id="rId1"/>
@@ -922,10 +922,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1347,7 +1343,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>4</v>

</xml_diff>